<commit_message>
[IMP] mrp_excel_bom_import_flat module: BoM type option added
</commit_message>
<xml_diff>
--- a/mrp_excel_bom_import_flat/data/import_flat_bom.xlsx
+++ b/mrp_excel_bom_import_flat/data/import_flat_bom.xlsx
@@ -20,9 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t xml:space="preserve">Types:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacture this product</t>
+  </si>
   <si>
     <t xml:space="preserve">BoM Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kit</t>
   </si>
   <si>
     <t xml:space="preserve">Product</t>
@@ -68,23 +80,35 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEDCE6"/>
+        <bgColor rgb="FFDEE6EF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDE8CB"/>
+        <bgColor rgb="FFDEE7E5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE7E5"/>
         <bgColor rgb="FFDEE6EF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDEE6EF"/>
-        <bgColor rgb="FFDDE8CB"/>
+        <bgColor rgb="FFDEE7E5"/>
       </patternFill>
     </fill>
   </fills>
@@ -129,16 +153,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,7 +224,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDEDCE6"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -190,7 +234,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDEE7E5"/>
       <rgbColor rgb="FFDDE8CB"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -223,31 +267,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AMJ5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.98"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
     </row>
-    <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
+    <row r="5" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="ALR5" s="0"/>
       <c r="ALS5" s="0"/>

</xml_diff>